<commit_message>
Add updated network performance numbers
</commit_message>
<xml_diff>
--- a/ai84net5 Performance.xlsx
+++ b/ai84net5 Performance.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robert.muchsel/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robert.muchsel/Documents/Source/ai84/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE135437-B810-BA43-836F-190E8FE4F0C6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D22FB2-99C5-024C-BF65-D57AB32FF3FA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11580" yWindow="5460" windowWidth="28040" windowHeight="17440" xr2:uid="{F15CDCCD-3FBD-5C4A-8D4D-282F3AF8325E}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="13">
   <si>
     <t>FashionMNIST</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>ai85 quant</t>
+  </si>
+  <si>
+    <t>With clamping FC layer:</t>
   </si>
 </sst>
 </file>
@@ -73,7 +76,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -124,7 +127,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22171EFF-A795-5C4A-885A-DA5D8DE0DBAF}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -548,6 +551,101 @@
       </c>
       <c r="E9" s="3"/>
     </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="3">
+        <v>99.4</v>
+      </c>
+      <c r="C15" s="3">
+        <v>99.6</v>
+      </c>
+      <c r="D15" s="3">
+        <v>99.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="3">
+        <v>92.3</v>
+      </c>
+      <c r="C16" s="3">
+        <v>92.1</v>
+      </c>
+      <c r="D16" s="3">
+        <v>91.7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="3">
+        <v>82.6</v>
+      </c>
+      <c r="C17" s="3">
+        <v>82</v>
+      </c>
+      <c r="D17" s="3">
+        <v>82.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="3">
+        <v>82.7</v>
+      </c>
+      <c r="C18" s="3">
+        <v>82.1</v>
+      </c>
+      <c r="D18" s="3">
+        <v>31.1</v>
+      </c>
+      <c r="E18" s="3">
+        <v>81.599999999999994</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>